<commit_message>
Formated BOM for main PCB
</commit_message>
<xml_diff>
--- a/Betula/Betula_Main/BOM_Betula_Main.xlsx
+++ b/Betula/Betula_Main/BOM_Betula_Main.xlsx
@@ -40,19 +40,37 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">R9,R12,R10,R6,R11,R5,R1,R7,R8,R39,R19,R42,R28,R33,R47,R44,R25,R54,R15,R26,R30,R17,R18,R40,R31,R22,R53,R32,R45,R20,R16,R36,R51,R49,R14,R23,R24,R29,R46,R27,R37,R48,R43,R34,R38,R50,R35,R52,R21,R41</t>
+    <t xml:space="preserve">R3,R4,R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-07220KL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1,R5,R6,R7,R8,R9,R10,R11,R12,R14,R15,R16,R17,R18,R19,R20,R21,R22,R23,R24,R25,R26,R27,R28,R29,R30,R31,R32,R33,R34,R35,R36,R37,R38,R39,R40,R41,R42,R43,R44,R45,R46,R47,R48,R49,R50,R51,R52,R53,R54</t>
   </si>
   <si>
     <t xml:space="preserve">5k6</t>
   </si>
   <si>
-    <t xml:space="preserve">R_0603</t>
-  </si>
-  <si>
     <t xml:space="preserve">603-RC0603FR-075K6L </t>
   </si>
   <si>
-    <t xml:space="preserve">R55,R58,R61,R60,R57,R59,R56</t>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2k2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-072K2L </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R55,R56,R57,R58,R59,R60,R61</t>
   </si>
   <si>
     <t xml:space="preserve">47R</t>
@@ -61,24 +79,6 @@
     <t xml:space="preserve">603-RC0603FR-0747RL </t>
   </si>
   <si>
-    <t xml:space="preserve">R4,R13,R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">220k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-07220KL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2k2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-072K2L </t>
-  </si>
-  <si>
     <t xml:space="preserve">RV1,RV2,RV3,RV4,RV5,RV6,RV7,RV8</t>
   </si>
   <si>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">652-TC33X-2-501E</t>
   </si>
   <si>
-    <t xml:space="preserve">C12,C26,C20,C27,C52,C55,C4,C14,C11,C23,C18,C53,C30,C3,C33,C29,C7,C6,C10,C54,C21,C72,C60,C70,C69,C63,C67,C71</t>
+    <t xml:space="preserve">C3,C4,C6,C7,C10,C11,C12,C14,C18,C20,C21,C23,C26,C27,C29,C30,C33,C52,C53,C54,C55,C60,C63,C67,C69,C70,C71,C72</t>
   </si>
   <si>
     <t xml:space="preserve">100n</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">80-C0603C104J5RACLR </t>
   </si>
   <si>
-    <t xml:space="preserve">C38,C40,C39</t>
+    <t xml:space="preserve">C38,C39,C40</t>
   </si>
   <si>
     <t xml:space="preserve">22u</t>
@@ -115,25 +115,7 @@
     <t xml:space="preserve">187-CL21A226MOCLRNC </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C16,C1,C22,C32,C25,C45,C28,C2,C31,C24,C9,C19,C15,C5,C17,C13,C8,C74,C73,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C36,C34,C35,C68</t>
-    </r>
+    <t xml:space="preserve">C1,C2,C5,C8,C9,C13,C15,C16,C17,C19,C22,C24,C25,C28,C31,C32,C34,C35,C36,C45,C68,C73,C74</t>
   </si>
   <si>
     <t xml:space="preserve">10u</t>
@@ -151,7 +133,7 @@
     <t xml:space="preserve">603-CC603KRX5R8BB105 </t>
   </si>
   <si>
-    <t xml:space="preserve">C43,C42,C41,C48,C50,C44,C49,C51,C59,C64,C62,C61,C56,C57,C58,C65</t>
+    <t xml:space="preserve">C41,C42,C43,C44,C48,C49,C50,C51,C56,C57,C58,C59,C61,C62,C64,C65</t>
   </si>
   <si>
     <t xml:space="preserve">330p</t>
@@ -196,7 +178,7 @@
     <t xml:space="preserve">595-TL062CDR</t>
   </si>
   <si>
-    <t xml:space="preserve">U3,U1,U2,U4</t>
+    <t xml:space="preserve">U1,U2,U3,U4</t>
   </si>
   <si>
     <t xml:space="preserve">PCM1803A</t>
@@ -256,7 +238,7 @@
     <t xml:space="preserve">U5</t>
   </si>
   <si>
-    <t xml:space="preserve">LDK320AU50R </t>
+    <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">SOT89 </t>
@@ -265,7 +247,7 @@
     <t xml:space="preserve">511-LDK320AU50R </t>
   </si>
   <si>
-    <t xml:space="preserve">U12,U16,U15,U13</t>
+    <t xml:space="preserve">U12,U13,U15,U16</t>
   </si>
   <si>
     <t xml:space="preserve">TLV9354</t>
@@ -361,7 +343,7 @@
     <t xml:space="preserve">2x2 Pin Header Socket</t>
   </si>
   <si>
-    <t xml:space="preserve">Conn_02x05_Odd_Even</t>
+    <t xml:space="preserve">02x05 Power connector</t>
   </si>
 </sst>
 </file>
@@ -371,7 +353,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,12 +375,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -456,7 +432,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,7 +628,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,71 +660,71 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed DC/DC converters to R-78Kx, updated to v1.5.2
</commit_message>
<xml_diff>
--- a/Betula/Betula_Main/BOM_Betula_Main.xlsx
+++ b/Betula/Betula_Main/BOM_Betula_Main.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
   <si>
     <t xml:space="preserve">Reference(s)</t>
   </si>
@@ -166,6 +166,18 @@
     <t xml:space="preserve">696-SSLLX3044SRC/D</t>
   </si>
   <si>
+    <t xml:space="preserve">D3, D4,D5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1N5819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD-123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">621-1N5819HW-F </t>
+  </si>
+  <si>
     <t xml:space="preserve">U6</t>
   </si>
   <si>
@@ -307,31 +319,31 @@
     <t xml:space="preserve">621-DMN3030LSS-13</t>
   </si>
   <si>
-    <t xml:space="preserve">PS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PXO7806-500-M-TR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-PXO7806-500-M-TR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PXO7803-500-M-TR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-PXO7803-500-M-TR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PXO7805-500-M-TR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-PXO7805-500-M-TR </t>
+    <t xml:space="preserve">U17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-78K6.5-0.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">919-R-78K6.5-0.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-78K5.0-0.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">919-R-78K5.0-0.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-78K63.3-0.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">919-R-78K3.3-0.5 </t>
   </si>
   <si>
     <t xml:space="preserve">15x1 Pin Header Socket</t>
@@ -419,7 +431,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -434,6 +446,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -625,10 +641,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -867,20 +883,20 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E16" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -889,7 +905,7 @@
         <v>52</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>53</v>
@@ -906,7 +922,7 @@
         <v>56</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>57</v>
@@ -931,7 +947,7 @@
       <c r="D20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -948,7 +964,7 @@
       <c r="D21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -965,25 +981,25 @@
       <c r="D22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>63</v>
+      <c r="E22" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,7 +1007,7 @@
         <v>75</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>76</v>
@@ -1002,22 +1018,19 @@
       <c r="E24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>82</v>
@@ -1037,26 +1050,29 @@
         <v>85</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1071,76 +1087,85 @@
         <v>93</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>97</v>
+      <c r="E30" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C35" s="1" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>106</v>
+      <c r="C37" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1148,7 +1173,15 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>